<commit_message>
income velocity temporarily, but time series made
</commit_message>
<xml_diff>
--- a/termpaper/styrrantan-effektiv.xlsx
+++ b/termpaper/styrrantan-effektiv.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1816B20E-92E4-490B-BC53-EB519E989BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9990"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporäntan per förändring" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,7 +86,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -305,12 +306,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -326,447 +327,447 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>38743</v>
+        <v>40961</v>
       </c>
       <c r="B2" s="3">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>38778</v>
+        <v>41024</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>38840</v>
+        <v>41101</v>
       </c>
       <c r="B4" s="3">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>38890</v>
+        <v>41164</v>
       </c>
       <c r="B5" s="3">
-        <v>2.25</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>38967</v>
+        <v>41213</v>
       </c>
       <c r="B6" s="3">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>39023</v>
+        <v>41262</v>
       </c>
       <c r="B7" s="3">
-        <v>2.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>39072</v>
+        <v>41325</v>
       </c>
       <c r="B8" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>39135</v>
+        <v>41388</v>
       </c>
       <c r="B9" s="3">
-        <v>3.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>39176</v>
+        <v>41465</v>
       </c>
       <c r="B10" s="3">
-        <v>3.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>39211</v>
+        <v>41528</v>
       </c>
       <c r="B11" s="3">
-        <v>3.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>39260</v>
+        <v>41577</v>
       </c>
       <c r="B12" s="3">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>39337</v>
+        <v>41626</v>
       </c>
       <c r="B13" s="3">
-        <v>3.75</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>39386</v>
+        <v>41689</v>
       </c>
       <c r="B14" s="3">
-        <v>3.75</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>39436</v>
+        <v>41745</v>
       </c>
       <c r="B15" s="3">
-        <v>4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>39498</v>
+        <v>41829</v>
       </c>
       <c r="B16" s="3">
-        <v>4.25</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>39568</v>
+        <v>41892</v>
       </c>
       <c r="B17" s="3">
-        <v>4.25</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>39638</v>
+        <v>41941</v>
       </c>
       <c r="B18" s="3">
-        <v>4.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>39701</v>
+        <v>41990</v>
       </c>
       <c r="B19" s="3">
-        <v>4.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>39736</v>
+        <v>42053</v>
       </c>
       <c r="B20" s="3">
-        <v>4.25</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>39750</v>
+        <v>42088</v>
       </c>
       <c r="B21" s="3">
-        <v>3.75</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>39792</v>
+        <v>42130</v>
       </c>
       <c r="B22" s="3">
-        <v>2</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>39862</v>
+        <v>42193</v>
       </c>
       <c r="B23" s="3">
-        <v>1</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>39925</v>
+        <v>42256</v>
       </c>
       <c r="B24" s="3">
-        <v>0.5</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>40002</v>
+        <v>42312</v>
       </c>
       <c r="B25" s="3">
-        <v>0.25</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>40065</v>
+        <v>42354</v>
       </c>
       <c r="B26" s="3">
-        <v>0.25</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>40114</v>
+        <v>42417</v>
       </c>
       <c r="B27" s="3">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>40170</v>
+        <v>42487</v>
       </c>
       <c r="B28" s="3">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>40226</v>
+        <v>42564</v>
       </c>
       <c r="B29" s="3">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>40289</v>
+        <v>42627</v>
       </c>
       <c r="B30" s="3">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>40366</v>
+        <v>42676</v>
       </c>
       <c r="B31" s="3">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>40429</v>
+        <v>42732</v>
       </c>
       <c r="B32" s="3">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>40478</v>
+        <v>42788</v>
       </c>
       <c r="B33" s="3">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>40534</v>
+        <v>42858</v>
       </c>
       <c r="B34" s="3">
-        <v>1.25</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>40590</v>
+        <v>42921</v>
       </c>
       <c r="B35" s="3">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>40660</v>
+        <v>42991</v>
       </c>
       <c r="B36" s="3">
-        <v>1.75</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>40730</v>
+        <v>43040</v>
       </c>
       <c r="B37" s="3">
-        <v>2</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>40800</v>
+        <v>43103</v>
       </c>
       <c r="B38" s="3">
-        <v>2</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>40849</v>
+        <v>43152</v>
       </c>
       <c r="B39" s="3">
-        <v>2</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>40898</v>
+        <v>43222</v>
       </c>
       <c r="B40" s="3">
-        <v>1.75</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>40961</v>
+        <v>43285</v>
       </c>
       <c r="B41" s="3">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>41024</v>
+        <v>43355</v>
       </c>
       <c r="B42" s="3">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>41101</v>
+        <v>43404</v>
       </c>
       <c r="B43" s="3">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>41164</v>
+        <v>43474</v>
       </c>
       <c r="B44" s="3">
-        <v>1.25</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>41213</v>
+        <v>43516</v>
       </c>
       <c r="B45" s="3">
-        <v>1.25</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>41262</v>
+        <v>43593</v>
       </c>
       <c r="B46" s="3">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>41325</v>
+        <v>43656</v>
       </c>
       <c r="B47" s="3">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>41388</v>
+        <v>43719</v>
       </c>
       <c r="B48" s="3">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>41465</v>
+        <v>43768</v>
       </c>
       <c r="B49" s="3">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>41528</v>
+        <v>43838</v>
       </c>
       <c r="B50" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>41577</v>
+        <v>43880</v>
       </c>
       <c r="B51" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>41626</v>
+        <v>43908</v>
       </c>
       <c r="B52" s="3">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>41689</v>
+        <v>43950</v>
       </c>
       <c r="B53" s="3">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>41745</v>
+        <v>44020</v>
       </c>
       <c r="B54" s="3">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>41829</v>
+        <v>44097</v>
       </c>
       <c r="B55" s="3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>41892</v>
+        <v>44167</v>
       </c>
       <c r="B56" s="3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>41941</v>
+        <v>44244</v>
       </c>
       <c r="B57" s="3">
         <v>0</v>
@@ -774,7 +775,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>41990</v>
+        <v>44314</v>
       </c>
       <c r="B58" s="3">
         <v>0</v>
@@ -782,394 +783,66 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>42053</v>
+        <v>44384</v>
       </c>
       <c r="B59" s="3">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>42088</v>
+        <v>44461</v>
       </c>
       <c r="B60" s="3">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>42130</v>
+        <v>44531</v>
       </c>
       <c r="B61" s="3">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>42193</v>
+        <v>44608</v>
       </c>
       <c r="B62" s="3">
-        <v>-0.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>42256</v>
+        <v>44685</v>
       </c>
       <c r="B63" s="3">
-        <v>-0.35</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>42312</v>
+        <v>44748</v>
       </c>
       <c r="B64" s="3">
-        <v>-0.35</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>42354</v>
+        <v>44825</v>
       </c>
       <c r="B65" s="3">
-        <v>-0.35</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>42417</v>
-      </c>
-      <c r="B66" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>42487</v>
-      </c>
-      <c r="B67" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
-        <v>42564</v>
-      </c>
-      <c r="B68" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>42627</v>
-      </c>
-      <c r="B69" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>42676</v>
-      </c>
-      <c r="B70" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>42732</v>
-      </c>
-      <c r="B71" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
-        <v>42788</v>
-      </c>
-      <c r="B72" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
-        <v>42858</v>
-      </c>
-      <c r="B73" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
-        <v>42921</v>
-      </c>
-      <c r="B74" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
-        <v>42991</v>
-      </c>
-      <c r="B75" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
-        <v>43040</v>
-      </c>
-      <c r="B76" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
-        <v>43103</v>
-      </c>
-      <c r="B77" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
-        <v>43152</v>
-      </c>
-      <c r="B78" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
-        <v>43222</v>
-      </c>
-      <c r="B79" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
-        <v>43285</v>
-      </c>
-      <c r="B80" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>43355</v>
-      </c>
-      <c r="B81" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
-        <v>43404</v>
-      </c>
-      <c r="B82" s="3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
-        <v>43474</v>
-      </c>
-      <c r="B83" s="3">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
-        <v>43516</v>
-      </c>
-      <c r="B84" s="3">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
-        <v>43593</v>
-      </c>
-      <c r="B85" s="3">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
-        <v>43656</v>
-      </c>
-      <c r="B86" s="3">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
-        <v>43719</v>
-      </c>
-      <c r="B87" s="3">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
-        <v>43768</v>
-      </c>
-      <c r="B88" s="3">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
-        <v>43838</v>
-      </c>
-      <c r="B89" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>43880</v>
-      </c>
-      <c r="B90" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
-        <v>43908</v>
-      </c>
-      <c r="B91" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>43950</v>
-      </c>
-      <c r="B92" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
-        <v>44020</v>
-      </c>
-      <c r="B93" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
-        <v>44097</v>
-      </c>
-      <c r="B94" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
-        <v>44167</v>
-      </c>
-      <c r="B95" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
-        <v>44244</v>
-      </c>
-      <c r="B96" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
-        <v>44314</v>
-      </c>
-      <c r="B97" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
-        <v>44384</v>
-      </c>
-      <c r="B98" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
-        <v>44461</v>
-      </c>
-      <c r="B99" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
-        <v>44531</v>
-      </c>
-      <c r="B100" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
-        <v>44608</v>
-      </c>
-      <c r="B101" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
-        <v>44685</v>
-      </c>
-      <c r="B102" s="3">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
-        <v>44748</v>
-      </c>
-      <c r="B103" s="3">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
-        <v>44825</v>
-      </c>
-      <c r="B104" s="3">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
         <v>44895</v>
       </c>
-      <c r="B105" s="4">
+      <c r="B66" s="4">
         <v>2.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
-        <v>44972</v>
-      </c>
-      <c r="B106" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
-        <v>45049</v>
-      </c>
-      <c r="B107" s="3">
-        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>